<commit_message>
almost finalised numbers and figures
</commit_message>
<xml_diff>
--- a/bigTableOfDoom.xlsx
+++ b/bigTableOfDoom.xlsx
@@ -489,10 +489,10 @@
     <xf numFmtId="164" fontId="6" fillId="3" borderId="3" xfId="5" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="7" fillId="8" borderId="0" xfId="10" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="3"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="3" applyAlignment="1"/>
-    <xf numFmtId="10" fontId="7" fillId="8" borderId="0" xfId="10" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="20% - Accent2" xfId="8" builtinId="34"/>
@@ -510,17 +510,7 @@
     <cellStyle name="Note" xfId="6" builtinId="10"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <font>
         <color theme="0"/>
@@ -804,8 +794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48:Q52"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -814,12 +804,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="18" thickBot="1">
-      <c r="A1" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
+      <c r="A1" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
     </row>
     <row r="2" spans="1:18" ht="17.25" thickTop="1"/>
     <row r="3" spans="1:18">
@@ -838,16 +828,16 @@
     </row>
     <row r="4" spans="1:18">
       <c r="A4" s="1">
-        <v>544</v>
+        <v>199</v>
       </c>
       <c r="B4" s="1">
-        <v>358</v>
+        <v>144</v>
       </c>
       <c r="C4" s="1">
-        <v>165</v>
+        <v>44</v>
       </c>
       <c r="D4" s="1">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:18">
@@ -856,15 +846,15 @@
       </c>
       <c r="B5" s="20">
         <f>ndd/ntot</f>
-        <v>0.65808823529411764</v>
+        <v>0.72361809045226133</v>
       </c>
       <c r="C5" s="20">
         <f>npd/ntot</f>
-        <v>0.30330882352941174</v>
+        <v>0.22110552763819097</v>
       </c>
       <c r="D5" s="20">
         <f>npp/ntot</f>
-        <v>3.860294117647059E-2</v>
+        <v>5.5276381909547742E-2</v>
       </c>
     </row>
     <row r="6" spans="1:18">
@@ -873,15 +863,15 @@
       </c>
       <c r="B6" s="20">
         <f>SQRT(ndd)/ntot</f>
-        <v>3.4781043986074456E-2</v>
+        <v>6.030150753768844E-2</v>
       </c>
       <c r="C6" s="20">
         <f>SQRT(npd)/ntot</f>
-        <v>2.3612559887252076E-2</v>
+        <v>3.3332912465883414E-2</v>
       </c>
       <c r="D6" s="20">
         <f>SQRT(npp)/ntot</f>
-        <v>8.4238523804335292E-3</v>
+        <v>1.6666456232941707E-2</v>
       </c>
     </row>
     <row r="7" spans="1:18">
@@ -891,11 +881,11 @@
       <c r="B7" s="10"/>
       <c r="C7" s="20">
         <f>ppd/(1-pdd)</f>
-        <v>0.88709677419354827</v>
+        <v>0.80000000000000016</v>
       </c>
       <c r="D7" s="20">
         <f>ppp/(1-pdd)</f>
-        <v>0.11290322580645161</v>
+        <v>0.20000000000000004</v>
       </c>
     </row>
     <row r="9" spans="1:18">
@@ -917,16 +907,16 @@
     </row>
     <row r="10" spans="1:18">
       <c r="A10" s="1">
-        <v>343</v>
+        <v>462</v>
       </c>
       <c r="B10" s="1">
-        <v>246</v>
+        <v>341</v>
       </c>
       <c r="C10" s="1">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="D10" s="1">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="E10" s="1">
         <v>13</v>
@@ -938,28 +928,28 @@
       </c>
       <c r="B11" s="20">
         <f>B10/dtot</f>
-        <v>0.71720116618075802</v>
+        <v>0.73809523809523814</v>
       </c>
       <c r="C11" s="20">
         <f>C10/dtot</f>
-        <v>0.12536443148688048</v>
+        <v>0.10606060606060606</v>
       </c>
       <c r="D11" s="20">
         <f>D10/dtot</f>
-        <v>0.119533527696793</v>
+        <v>0.12770562770562771</v>
       </c>
       <c r="E11" s="20">
         <f>E10/dtot</f>
-        <v>3.7900874635568516E-2</v>
+        <v>2.813852813852814E-2</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="18" thickBot="1">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="23"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
     </row>
     <row r="15" spans="1:18" ht="17.25" thickTop="1"/>
     <row r="16" spans="1:18">
@@ -1352,20 +1342,20 @@
       </c>
     </row>
     <row r="25" spans="1:18" ht="18" thickBot="1">
-      <c r="A25" s="23" t="s">
+      <c r="A25" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="B25" s="23"/>
-      <c r="C25" s="23"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="23"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
     </row>
     <row r="26" spans="1:18" ht="17.25" thickTop="1"/>
     <row r="27" spans="1:18" ht="17.25" thickBot="1">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="24"/>
+      <c r="B27" s="25"/>
       <c r="C27" s="2" t="s">
         <v>13</v>
       </c>
@@ -1419,67 +1409,67 @@
       <c r="B28" s="5"/>
       <c r="C28" s="6">
         <f>ppp</f>
-        <v>3.860294117647059E-2</v>
+        <v>5.5276381909547742E-2</v>
       </c>
       <c r="D28" s="6">
         <f>ppd*prph</f>
-        <v>0.21753344194820784</v>
+        <v>0.16319693706628383</v>
       </c>
       <c r="E28" s="6">
         <f>ppd*pama</f>
-        <v>3.802413822671926E-2</v>
+        <v>2.3450586264656618E-2</v>
       </c>
       <c r="F28" s="6">
         <f>ppd*pbip</f>
-        <v>3.625557365803464E-2</v>
+        <v>2.8236420196219195E-2</v>
       </c>
       <c r="G28" s="6">
         <f>ppd*pmul</f>
-        <v>1.1495669696450009E-2</v>
+        <v>6.2215841110313478E-3</v>
       </c>
       <c r="H28" s="6">
         <f>pdd*prph*prph</f>
-        <v>0.3385057896544707</v>
+        <v>0.39421597784842588</v>
       </c>
       <c r="I28" s="6">
         <f>pdd*prph*pama*2</f>
-        <v>0.11833942239953041</v>
+        <v>0.11329374143444497</v>
       </c>
       <c r="J28" s="6">
         <f>pdd*prph*pbip*2</f>
-        <v>0.11283526321815689</v>
+        <v>0.13641491315576026</v>
       </c>
       <c r="K28" s="6">
         <f>pdd*prph*pmul*2</f>
-        <v>3.5777034678927795E-2</v>
+        <v>3.0057523237709889E-2</v>
       </c>
       <c r="L28" s="6">
         <f>pdd*pama*pama</f>
-        <v>1.034267309589392E-2</v>
+        <v>8.1398729183105624E-3</v>
       </c>
       <c r="M28" s="6">
         <f>pdd*pama*pbip*2</f>
-        <v>1.9723237066588403E-2</v>
+        <v>1.9602142946135638E-2</v>
       </c>
       <c r="N28" s="6">
         <f>pdd*pama*pmul*2</f>
-        <v>6.2537093137963237E-3</v>
+        <v>4.3191162423688693E-3</v>
       </c>
       <c r="O28" s="6">
         <f>pdd*pbip*pbip</f>
-        <v>9.402938601513075E-3</v>
+        <v>1.1801290141040843E-2</v>
       </c>
       <c r="P28" s="6">
         <f>pdd*pbip*pmul*2</f>
-        <v>5.9628391131546334E-3</v>
+        <v>5.2005685367298637E-3</v>
       </c>
       <c r="Q28" s="6">
         <f>pdd*pmul*pmul</f>
-        <v>9.4532815208549063E-4</v>
+        <v>5.7294399133464601E-4</v>
       </c>
       <c r="R28" s="3">
         <f>SUM(C28:Q28)</f>
-        <v>0.99999999999999989</v>
+        <v>1.0000000000000002</v>
       </c>
     </row>
     <row r="29" spans="1:18">
@@ -1488,67 +1478,67 @@
       </c>
       <c r="B29" s="6">
         <f>ppp_</f>
-        <v>0.11290322580645161</v>
+        <v>0.20000000000000004</v>
       </c>
       <c r="C29" s="7">
         <f t="shared" ref="C29:Q33" si="2">C$28*$B29</f>
-        <v>4.3583965844402276E-3</v>
+        <v>1.105527638190955E-2</v>
       </c>
       <c r="D29" s="7">
         <f t="shared" si="2"/>
-        <v>2.4560227316733144E-2</v>
+        <v>3.2639387413256775E-2</v>
       </c>
       <c r="E29" s="7">
         <f t="shared" si="2"/>
-        <v>4.2930478643070135E-3</v>
+        <v>4.6901172529313249E-3</v>
       </c>
       <c r="F29" s="7">
         <f t="shared" si="2"/>
-        <v>4.0933712194555234E-3</v>
+        <v>5.6472840392438398E-3</v>
       </c>
       <c r="G29" s="7">
         <f t="shared" si="2"/>
-        <v>1.2978981915346783E-3</v>
+        <v>1.2443168222062697E-3</v>
       </c>
       <c r="H29" s="7">
         <f t="shared" si="2"/>
-        <v>3.8218395606149917E-2</v>
+        <v>7.8843195569685193E-2</v>
       </c>
       <c r="I29" s="7">
         <f t="shared" si="2"/>
-        <v>1.336090252897924E-2</v>
+        <v>2.2658748286888998E-2</v>
       </c>
       <c r="J29" s="7">
         <f t="shared" si="2"/>
-        <v>1.2739465202049971E-2</v>
+        <v>2.7282982631152058E-2</v>
       </c>
       <c r="K29" s="7">
         <f t="shared" si="2"/>
-        <v>4.0393426250402344E-3</v>
+        <v>6.0115046475419792E-3</v>
       </c>
       <c r="L29" s="7">
         <f t="shared" si="2"/>
-        <v>1.1677211559880231E-3</v>
+        <v>1.6279745836621127E-3</v>
       </c>
       <c r="M29" s="7">
         <f t="shared" si="2"/>
-        <v>2.2268170881632066E-3</v>
+        <v>3.9204285892271281E-3</v>
       </c>
       <c r="N29" s="7">
         <f t="shared" si="2"/>
-        <v>7.060639547834559E-4</v>
+        <v>8.63823248473774E-4</v>
       </c>
       <c r="O29" s="7">
         <f t="shared" si="2"/>
-        <v>1.061622100170831E-3</v>
+        <v>2.3602580282081689E-3</v>
       </c>
       <c r="P29" s="7">
         <f t="shared" si="2"/>
-        <v>6.7322377084003929E-4</v>
+        <v>1.0401137073459729E-3</v>
       </c>
       <c r="Q29" s="7">
         <f t="shared" si="2"/>
-        <v>1.0673059781610378E-4</v>
+        <v>1.1458879826692922E-4</v>
       </c>
     </row>
     <row r="30" spans="1:18">
@@ -1557,67 +1547,67 @@
       </c>
       <c r="B30" s="6">
         <f>ppd_*prph</f>
-        <v>0.63622684096680138</v>
+        <v>0.5904761904761906</v>
       </c>
       <c r="C30" s="7">
         <f t="shared" si="2"/>
-        <v>2.4560227316733144E-2</v>
+        <v>3.2639387413256768E-2</v>
       </c>
       <c r="D30" s="7">
         <f t="shared" si="2"/>
-        <v>0.13840061457534336</v>
+        <v>9.6363905696281893E-2</v>
       </c>
       <c r="E30" s="7">
         <f t="shared" si="2"/>
-        <v>2.4191977344470587E-2</v>
+        <v>1.384701284198772E-2</v>
       </c>
       <c r="F30" s="7">
         <f t="shared" si="2"/>
-        <v>2.3066769095890557E-2</v>
+        <v>1.6672933830148482E-2</v>
       </c>
       <c r="G30" s="7">
         <f t="shared" si="2"/>
-        <v>7.3138536157701774E-3</v>
+        <v>3.6736972846089871E-3</v>
       </c>
       <c r="H30" s="7">
         <f t="shared" si="2"/>
-        <v>0.21536646920083646</v>
+        <v>0.23277514882478487</v>
       </c>
       <c r="I30" s="7">
         <f t="shared" si="2"/>
-        <v>7.5290716875089161E-2</v>
+        <v>6.6897256847005621E-2</v>
       </c>
       <c r="J30" s="7">
         <f t="shared" si="2"/>
-        <v>7.1788823066945479E-2</v>
+        <v>8.0549758244353703E-2</v>
       </c>
       <c r="K30" s="7">
         <f t="shared" si="2"/>
-        <v>2.2762309752933932E-2</v>
+        <v>1.7748251816552509E-2</v>
       </c>
       <c r="L30" s="7">
         <f t="shared" si="2"/>
-        <v>6.5802862309529159E-3</v>
+        <v>4.8064011517643329E-3</v>
       </c>
       <c r="M30" s="7">
         <f t="shared" si="2"/>
-        <v>1.2548452812514863E-2</v>
+        <v>1.1574598692003902E-2</v>
       </c>
       <c r="N30" s="7">
         <f t="shared" si="2"/>
-        <v>3.978777721041298E-3</v>
+        <v>2.5503353050178091E-3</v>
       </c>
       <c r="O30" s="7">
         <f t="shared" si="2"/>
-        <v>5.9824019222454571E-3</v>
+        <v>6.9683808451860233E-3</v>
       </c>
       <c r="P30" s="7">
         <f t="shared" si="2"/>
-        <v>3.7937182921556557E-3</v>
+        <v>3.0708118978785867E-3</v>
       </c>
       <c r="Q30" s="7">
         <f t="shared" si="2"/>
-        <v>6.0144314387833569E-4</v>
+        <v>3.3830978535950531E-4</v>
       </c>
     </row>
     <row r="31" spans="1:18">
@@ -1626,67 +1616,67 @@
       </c>
       <c r="B31" s="6">
         <f>ppd_*pama</f>
-        <v>0.11121038277061976</v>
+        <v>8.4848484848484867E-2</v>
       </c>
       <c r="C31" s="7">
         <f t="shared" si="2"/>
-        <v>4.2930478643070126E-3</v>
+        <v>4.6901172529313249E-3</v>
       </c>
       <c r="D31" s="7">
         <f t="shared" si="2"/>
-        <v>2.4191977344470587E-2</v>
+        <v>1.3847012841987721E-2</v>
       </c>
       <c r="E31" s="7">
         <f t="shared" si="2"/>
-        <v>4.2286789667164036E-3</v>
+        <v>1.9897467133648044E-3</v>
       </c>
       <c r="F31" s="7">
         <f t="shared" si="2"/>
-        <v>4.0319962240784315E-3</v>
+        <v>2.3958174711943567E-3</v>
       </c>
       <c r="G31" s="7">
         <f t="shared" si="2"/>
-        <v>1.2784378271468197E-3</v>
+        <v>5.2789198517841753E-4</v>
       </c>
       <c r="H31" s="7">
         <f t="shared" si="2"/>
-        <v>3.7645358437544588E-2</v>
+        <v>3.344862842350281E-2</v>
       </c>
       <c r="I31" s="7">
         <f t="shared" si="2"/>
-        <v>1.316057246190583E-2</v>
+        <v>9.6128023035286659E-3</v>
       </c>
       <c r="J31" s="7">
         <f t="shared" si="2"/>
-        <v>1.2548452812514861E-2</v>
+        <v>1.1574598692003904E-2</v>
       </c>
       <c r="K31" s="7">
         <f t="shared" si="2"/>
-        <v>3.9787777210412972E-3</v>
+        <v>2.5503353050178095E-3</v>
       </c>
       <c r="L31" s="7">
         <f t="shared" si="2"/>
-        <v>1.1502126338657538E-3</v>
+        <v>6.9065588397786604E-4</v>
       </c>
       <c r="M31" s="7">
         <f t="shared" si="2"/>
-        <v>2.1934287436509718E-3</v>
+        <v>1.6632121287630242E-3</v>
       </c>
       <c r="N31" s="7">
         <f t="shared" si="2"/>
-        <v>6.9547740652347895E-4</v>
+        <v>3.664704690494799E-4</v>
       </c>
       <c r="O31" s="7">
         <f t="shared" si="2"/>
-        <v>1.0457044010429052E-3</v>
+        <v>1.0013215877246778E-3</v>
       </c>
       <c r="P31" s="7">
         <f t="shared" si="2"/>
-        <v>6.631296201735496E-4</v>
+        <v>4.4126036069223098E-4</v>
       </c>
       <c r="Q31" s="7">
         <f t="shared" si="2"/>
-        <v>1.0513030563727007E-4</v>
+        <v>4.8613429567788157E-5</v>
       </c>
     </row>
     <row r="32" spans="1:18">
@@ -1695,67 +1685,67 @@
       </c>
       <c r="B32" s="6">
         <f>ppd_*pbip</f>
-        <v>0.10603780682780023</v>
+        <v>0.10216450216450219</v>
       </c>
       <c r="C32" s="7">
         <f t="shared" si="2"/>
-        <v>4.0933712194555234E-3</v>
+        <v>5.6472840392438406E-3</v>
       </c>
       <c r="D32" s="7">
         <f t="shared" si="2"/>
-        <v>2.3066769095890557E-2</v>
+        <v>1.6672933830148482E-2</v>
       </c>
       <c r="E32" s="7">
         <f t="shared" si="2"/>
-        <v>4.0319962240784315E-3</v>
+        <v>2.3958174711943567E-3</v>
       </c>
       <c r="F32" s="7">
         <f t="shared" si="2"/>
-        <v>3.8444615159817599E-3</v>
+        <v>2.8847598122544293E-3</v>
       </c>
       <c r="G32" s="7">
         <f t="shared" si="2"/>
-        <v>1.218975602628363E-3</v>
+        <v>6.3562504337809464E-4</v>
       </c>
       <c r="H32" s="7">
         <f t="shared" si="2"/>
-        <v>3.5894411533472739E-2</v>
+        <v>4.0274879122176852E-2</v>
       </c>
       <c r="I32" s="7">
         <f t="shared" si="2"/>
-        <v>1.2548452812514861E-2</v>
+        <v>1.1574598692003906E-2</v>
       </c>
       <c r="J32" s="7">
         <f t="shared" si="2"/>
-        <v>1.1964803844490913E-2</v>
+        <v>1.3936761690372048E-2</v>
       </c>
       <c r="K32" s="7">
         <f t="shared" si="2"/>
-        <v>3.7937182921556553E-3</v>
+        <v>3.0708118978785871E-3</v>
       </c>
       <c r="L32" s="7">
         <f t="shared" si="2"/>
-        <v>1.0967143718254859E-3</v>
+        <v>8.316060643815122E-4</v>
       </c>
       <c r="M32" s="7">
         <f t="shared" si="2"/>
-        <v>2.0914088020858104E-3</v>
+        <v>2.0026431754493557E-3</v>
       </c>
       <c r="N32" s="7">
         <f t="shared" si="2"/>
-        <v>6.6312962017354971E-4</v>
+        <v>4.4126036069223093E-4</v>
       </c>
       <c r="O32" s="7">
         <f t="shared" si="2"/>
-        <v>9.9706698704090952E-4</v>
+        <v>1.2056729321582855E-3</v>
       </c>
       <c r="P32" s="7">
         <f t="shared" si="2"/>
-        <v>6.322863820259427E-4</v>
+        <v>5.3131349552738014E-4</v>
       </c>
       <c r="Q32" s="7">
         <f t="shared" si="2"/>
-        <v>1.0024052397972261E-4</v>
+        <v>5.8534537642846969E-5</v>
       </c>
     </row>
     <row r="33" spans="1:18">
@@ -1764,67 +1754,67 @@
       </c>
       <c r="B33" s="6">
         <f>ppd_*pmul</f>
-        <v>3.3621743628326907E-2</v>
+        <v>2.2510822510822516E-2</v>
       </c>
       <c r="C33" s="7">
         <f t="shared" si="2"/>
-        <v>1.2978981915346785E-3</v>
+        <v>1.2443168222062697E-3</v>
       </c>
       <c r="D33" s="7">
         <f t="shared" si="2"/>
-        <v>7.3138536157701783E-3</v>
+        <v>3.6736972846089875E-3</v>
       </c>
       <c r="E33" s="7">
         <f t="shared" si="2"/>
-        <v>1.2784378271468199E-3</v>
+        <v>5.2789198517841753E-4</v>
       </c>
       <c r="F33" s="7">
         <f t="shared" si="2"/>
-        <v>1.218975602628363E-3</v>
+        <v>6.3562504337809453E-4</v>
       </c>
       <c r="G33" s="7">
         <f t="shared" si="2"/>
-        <v>3.8650445936996879E-4</v>
+        <v>1.4005297565958017E-4</v>
       </c>
       <c r="H33" s="7">
         <f t="shared" si="2"/>
-        <v>1.1381154876466968E-2</v>
+        <v>8.8741259082762564E-3</v>
       </c>
       <c r="I33" s="7">
         <f t="shared" si="2"/>
-        <v>3.978777721041298E-3</v>
+        <v>2.5503353050178095E-3</v>
       </c>
       <c r="J33" s="7">
         <f t="shared" si="2"/>
-        <v>3.7937182921556557E-3</v>
+        <v>3.0708118978785867E-3</v>
       </c>
       <c r="K33" s="7">
         <f t="shared" si="2"/>
-        <v>1.2028862877566714E-3</v>
+        <v>6.7661957071901062E-4</v>
       </c>
       <c r="L33" s="7">
         <f t="shared" si="2"/>
-        <v>3.4773870326173953E-4</v>
+        <v>1.8323523452473998E-4</v>
       </c>
       <c r="M33" s="7">
         <f t="shared" si="2"/>
-        <v>6.6312962017354971E-4</v>
+        <v>4.4126036069223093E-4</v>
       </c>
       <c r="N33" s="7">
         <f t="shared" si="2"/>
-        <v>2.1026061127454019E-4</v>
+        <v>9.7226859135576301E-5</v>
       </c>
       <c r="O33" s="7">
         <f t="shared" si="2"/>
-        <v>3.1614319101297135E-4</v>
+        <v>2.6565674776369002E-4</v>
       </c>
       <c r="P33" s="7">
         <f t="shared" si="2"/>
-        <v>2.0048104795944525E-4</v>
+        <v>1.1706907528569393E-4</v>
       </c>
       <c r="Q33" s="7">
         <f t="shared" si="2"/>
-        <v>3.1783580774058393E-5</v>
+        <v>1.2897440497576449E-5</v>
       </c>
     </row>
     <row r="34" spans="1:18">
@@ -1833,78 +1823,78 @@
       </c>
       <c r="B34" s="3">
         <f>SUM(B29:B33)</f>
-        <v>0.99999999999999989</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="C34" s="15">
         <f>SUM(C29:C33)</f>
-        <v>3.8602941176470583E-2</v>
+        <v>5.5276381909547749E-2</v>
       </c>
       <c r="D34" s="15">
         <f t="shared" ref="D34:Q34" si="3">SUM(D29:D33)</f>
-        <v>0.21753344194820781</v>
+        <v>0.16319693706628385</v>
       </c>
       <c r="E34" s="15">
         <f t="shared" si="3"/>
-        <v>3.8024138226719253E-2</v>
+        <v>2.3450586264656622E-2</v>
       </c>
       <c r="F34" s="15">
         <f t="shared" si="3"/>
-        <v>3.6255573658034633E-2</v>
+        <v>2.8236420196219199E-2</v>
       </c>
       <c r="G34" s="15">
         <f t="shared" si="3"/>
-        <v>1.1495669696450007E-2</v>
+        <v>6.2215841110313478E-3</v>
       </c>
       <c r="H34" s="15">
         <f t="shared" si="3"/>
-        <v>0.33850578965447065</v>
+        <v>0.39421597784842599</v>
       </c>
       <c r="I34" s="15">
         <f t="shared" si="3"/>
-        <v>0.11833942239953039</v>
+        <v>0.11329374143444498</v>
       </c>
       <c r="J34" s="15">
         <f t="shared" si="3"/>
-        <v>0.11283526321815689</v>
+        <v>0.13641491315576029</v>
       </c>
       <c r="K34" s="15">
         <f t="shared" si="3"/>
-        <v>3.5777034678927795E-2</v>
+        <v>3.0057523237709896E-2</v>
       </c>
       <c r="L34" s="15">
         <f t="shared" si="3"/>
-        <v>1.0342673095893918E-2</v>
+        <v>8.1398729183105641E-3</v>
       </c>
       <c r="M34" s="15">
         <f t="shared" si="3"/>
-        <v>1.9723237066588403E-2</v>
+        <v>1.9602142946135642E-2</v>
       </c>
       <c r="N34" s="15">
         <f t="shared" si="3"/>
-        <v>6.2537093137963228E-3</v>
+        <v>4.3191162423688702E-3</v>
       </c>
       <c r="O34" s="15">
         <f t="shared" si="3"/>
-        <v>9.4029386015130716E-3</v>
+        <v>1.1801290141040846E-2</v>
       </c>
       <c r="P34" s="15">
         <f t="shared" si="3"/>
-        <v>5.9628391131546334E-3</v>
+        <v>5.2005685367298637E-3</v>
       </c>
       <c r="Q34" s="15">
         <f t="shared" si="3"/>
-        <v>9.4532815208549052E-4</v>
+        <v>5.7294399133464612E-4</v>
       </c>
       <c r="R34" s="3">
         <f>SUM(C29:Q33)</f>
-        <v>0.99999999999999989</v>
+        <v>1.0000000000000007</v>
       </c>
     </row>
     <row r="36" spans="1:18" ht="17.25" thickBot="1">
-      <c r="A36" s="24" t="s">
+      <c r="A36" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="B36" s="24"/>
+      <c r="B36" s="25"/>
       <c r="C36" s="2" t="s">
         <v>13</v>
       </c>
@@ -1957,63 +1947,63 @@
       </c>
       <c r="C37" s="9">
         <f t="shared" ref="C37:Q37" si="4">C29*total3</f>
-        <v>0.87603771347248571</v>
+        <v>2.2221105527638194</v>
       </c>
       <c r="D37" s="9">
         <f t="shared" si="4"/>
-        <v>4.9366056906633622</v>
+        <v>6.5605168700646121</v>
       </c>
       <c r="E37" s="9">
         <f t="shared" si="4"/>
-        <v>0.86290262072570967</v>
+        <v>0.94271356783919635</v>
       </c>
       <c r="F37" s="9">
         <f t="shared" si="4"/>
-        <v>0.82276761511056018</v>
+        <v>1.1351040918880118</v>
       </c>
       <c r="G37" s="9">
         <f t="shared" si="4"/>
-        <v>0.26087753649847034</v>
+        <v>0.25010768126346022</v>
       </c>
       <c r="H37" s="9">
         <f t="shared" si="4"/>
-        <v>7.6818975168361332</v>
+        <v>15.847482309506724</v>
       </c>
       <c r="I37" s="9">
         <f t="shared" si="4"/>
-        <v>2.685541408324827</v>
+        <v>4.554408405664689</v>
       </c>
       <c r="J37" s="9">
         <f t="shared" si="4"/>
-        <v>2.5606325056120443</v>
+        <v>5.4838795088615635</v>
       </c>
       <c r="K37" s="9">
         <f t="shared" si="4"/>
-        <v>0.81190786763308709</v>
+        <v>1.2083124341559379</v>
       </c>
       <c r="L37" s="9">
         <f t="shared" si="4"/>
-        <v>0.23471195235359266</v>
+        <v>0.32722289131608467</v>
       </c>
       <c r="M37" s="9">
         <f t="shared" si="4"/>
-        <v>0.44759023472080456</v>
+        <v>0.78800614643465272</v>
       </c>
       <c r="N37" s="9">
         <f t="shared" si="4"/>
-        <v>0.14191885491147463</v>
+        <v>0.17362847294322858</v>
       </c>
       <c r="O37" s="9">
         <f t="shared" si="4"/>
-        <v>0.21338604213433701</v>
+        <v>0.47441186366984195</v>
       </c>
       <c r="P37" s="9">
         <f t="shared" si="4"/>
-        <v>0.13531797793884789</v>
+        <v>0.20906285517654055</v>
       </c>
       <c r="Q37" s="9">
         <f t="shared" si="4"/>
-        <v>2.145285016103686E-2</v>
+        <v>2.3032348451652775E-2</v>
       </c>
     </row>
     <row r="38" spans="1:18">
@@ -2022,63 +2012,63 @@
       </c>
       <c r="C38" s="9">
         <f t="shared" ref="C38:Q38" si="5">C30*total3</f>
-        <v>4.9366056906633622</v>
+        <v>6.5605168700646104</v>
       </c>
       <c r="D38" s="9">
         <f t="shared" si="5"/>
-        <v>27.818523529644015</v>
+        <v>19.36914504495266</v>
       </c>
       <c r="E38" s="9">
         <f t="shared" si="5"/>
-        <v>4.8625874462385879</v>
+        <v>2.7832495812395317</v>
       </c>
       <c r="F38" s="9">
         <f t="shared" si="5"/>
-        <v>4.6364205882740022</v>
+        <v>3.351259699859845</v>
       </c>
       <c r="G38" s="9">
         <f t="shared" si="5"/>
-        <v>1.4700845767698056</v>
+        <v>0.73841315420640641</v>
       </c>
       <c r="H38" s="9">
         <f t="shared" si="5"/>
-        <v>43.288660309368126</v>
+        <v>46.787804913781756</v>
       </c>
       <c r="I38" s="9">
         <f t="shared" si="5"/>
-        <v>15.133434091892921</v>
+        <v>13.446348626248129</v>
       </c>
       <c r="J38" s="9">
         <f t="shared" si="5"/>
-        <v>14.429553436456041</v>
+        <v>16.190501407115093</v>
       </c>
       <c r="K38" s="9">
         <f t="shared" si="5"/>
-        <v>4.57522426033972</v>
+        <v>3.5673986151270545</v>
       </c>
       <c r="L38" s="9">
         <f t="shared" si="5"/>
-        <v>1.322637532421536</v>
+        <v>0.96608663150463092</v>
       </c>
       <c r="M38" s="9">
         <f t="shared" si="5"/>
-        <v>2.5222390153154874</v>
+        <v>2.3264943370927842</v>
       </c>
       <c r="N38" s="9">
         <f t="shared" si="5"/>
-        <v>0.79973432192930094</v>
+        <v>0.51261739630857961</v>
       </c>
       <c r="O38" s="9">
         <f t="shared" si="5"/>
-        <v>1.2024627863713369</v>
+        <v>1.4006445498823907</v>
       </c>
       <c r="P38" s="9">
         <f t="shared" si="5"/>
-        <v>0.76253737672328681</v>
+        <v>0.6172331914735959</v>
       </c>
       <c r="Q38" s="9">
         <f t="shared" si="5"/>
-        <v>0.12089007191954547</v>
+        <v>6.8000266857260572E-2</v>
       </c>
     </row>
     <row r="39" spans="1:18">
@@ -2087,63 +2077,63 @@
       </c>
       <c r="C39" s="9">
         <f t="shared" ref="C39:Q39" si="6">C31*total3</f>
-        <v>0.86290262072570956</v>
+        <v>0.94271356783919635</v>
       </c>
       <c r="D39" s="9">
         <f t="shared" si="6"/>
-        <v>4.8625874462385879</v>
+        <v>2.7832495812395321</v>
       </c>
       <c r="E39" s="9">
         <f t="shared" si="6"/>
-        <v>0.84996447230999717</v>
+        <v>0.39993908938632566</v>
       </c>
       <c r="F39" s="9">
         <f t="shared" si="6"/>
-        <v>0.81043124103976472</v>
+        <v>0.48155931171006572</v>
       </c>
       <c r="G39" s="9">
         <f t="shared" si="6"/>
-        <v>0.25696600325651076</v>
+        <v>0.10610628902086193</v>
       </c>
       <c r="H39" s="9">
         <f t="shared" si="6"/>
-        <v>7.5667170459464623</v>
+        <v>6.7231743131240647</v>
       </c>
       <c r="I39" s="9">
         <f t="shared" si="6"/>
-        <v>2.6452750648430721</v>
+        <v>1.9321732630092618</v>
       </c>
       <c r="J39" s="9">
         <f t="shared" si="6"/>
-        <v>2.522239015315487</v>
+        <v>2.3264943370927846</v>
       </c>
       <c r="K39" s="9">
         <f t="shared" si="6"/>
-        <v>0.79973432192930072</v>
+        <v>0.51261739630857972</v>
       </c>
       <c r="L39" s="9">
         <f t="shared" si="6"/>
-        <v>0.23119273940701651</v>
+        <v>0.13882183267955106</v>
       </c>
       <c r="M39" s="9">
         <f t="shared" si="6"/>
-        <v>0.44087917747384536</v>
+        <v>0.33430563788136786</v>
       </c>
       <c r="N39" s="9">
         <f t="shared" si="6"/>
-        <v>0.13979095871121927</v>
+        <v>7.3660564278945462E-2</v>
       </c>
       <c r="O39" s="9">
         <f t="shared" si="6"/>
-        <v>0.21018658460962394</v>
+        <v>0.20126563913266024</v>
       </c>
       <c r="P39" s="9">
         <f t="shared" si="6"/>
-        <v>0.13328905365488347</v>
+        <v>8.8693332499138425E-2</v>
       </c>
       <c r="Q39" s="9">
         <f t="shared" si="6"/>
-        <v>2.1131191433091282E-2</v>
+        <v>9.7712993431254194E-3</v>
       </c>
     </row>
     <row r="40" spans="1:18">
@@ -2152,63 +2142,63 @@
       </c>
       <c r="C40" s="9">
         <f t="shared" ref="C40:Q40" si="7">C32*total3</f>
-        <v>0.82276761511056018</v>
+        <v>1.135104091888012</v>
       </c>
       <c r="D40" s="9">
         <f t="shared" si="7"/>
-        <v>4.6364205882740022</v>
+        <v>3.351259699859845</v>
       </c>
       <c r="E40" s="9">
         <f t="shared" si="7"/>
-        <v>0.81043124103976472</v>
+        <v>0.48155931171006572</v>
       </c>
       <c r="F40" s="9">
         <f t="shared" si="7"/>
-        <v>0.77273676471233377</v>
+        <v>0.57983672226314031</v>
       </c>
       <c r="G40" s="9">
         <f t="shared" si="7"/>
-        <v>0.24501409612830097</v>
+        <v>0.12776063371899701</v>
       </c>
       <c r="H40" s="9">
         <f t="shared" si="7"/>
-        <v>7.2147767182280207</v>
+        <v>8.0952507035575465</v>
       </c>
       <c r="I40" s="9">
         <f t="shared" si="7"/>
-        <v>2.522239015315487</v>
+        <v>2.3264943370927851</v>
       </c>
       <c r="J40" s="9">
         <f t="shared" si="7"/>
-        <v>2.4049255727426733</v>
+        <v>2.8012890997647819</v>
       </c>
       <c r="K40" s="9">
         <f t="shared" si="7"/>
-        <v>0.7625373767232867</v>
+        <v>0.61723319147359601</v>
       </c>
       <c r="L40" s="9">
         <f t="shared" si="7"/>
-        <v>0.22043958873692268</v>
+        <v>0.16715281894068396</v>
       </c>
       <c r="M40" s="9">
         <f t="shared" si="7"/>
-        <v>0.42037316921924789</v>
+        <v>0.40253127826532048</v>
       </c>
       <c r="N40" s="9">
         <f t="shared" si="7"/>
-        <v>0.1332890536548835</v>
+        <v>8.8693332499138411E-2</v>
       </c>
       <c r="O40" s="9">
         <f t="shared" si="7"/>
-        <v>0.20041046439522281</v>
+        <v>0.2423402593638154</v>
       </c>
       <c r="P40" s="9">
         <f t="shared" si="7"/>
-        <v>0.12708956278721448</v>
+        <v>0.10679401260100341</v>
       </c>
       <c r="Q40" s="9">
         <f t="shared" si="7"/>
-        <v>2.0148345319924245E-2</v>
+        <v>1.1765442066212242E-2</v>
       </c>
     </row>
     <row r="41" spans="1:18">
@@ -2217,63 +2207,63 @@
       </c>
       <c r="C41" s="9">
         <f t="shared" ref="C41:Q42" si="8">C33*total3</f>
-        <v>0.2608775364984704</v>
+        <v>0.25010768126346022</v>
       </c>
       <c r="D41" s="9">
         <f t="shared" si="8"/>
-        <v>1.4700845767698059</v>
+        <v>0.73841315420640652</v>
       </c>
       <c r="E41" s="9">
         <f t="shared" si="8"/>
-        <v>0.25696600325651081</v>
+        <v>0.10610628902086193</v>
       </c>
       <c r="F41" s="9">
         <f t="shared" si="8"/>
-        <v>0.24501409612830097</v>
+        <v>0.12776063371899701</v>
       </c>
       <c r="G41" s="9">
         <f t="shared" si="8"/>
-        <v>7.7687396333363731E-2</v>
+        <v>2.8150648107575612E-2</v>
       </c>
       <c r="H41" s="9">
         <f t="shared" si="8"/>
-        <v>2.2876121301698604</v>
+        <v>1.7836993075635275</v>
       </c>
       <c r="I41" s="9">
         <f t="shared" si="8"/>
-        <v>0.79973432192930094</v>
+        <v>0.51261739630857972</v>
       </c>
       <c r="J41" s="9">
         <f t="shared" si="8"/>
-        <v>0.76253737672328681</v>
+        <v>0.6172331914735959</v>
       </c>
       <c r="K41" s="9">
         <f t="shared" si="8"/>
-        <v>0.24178014383909094</v>
+        <v>0.13600053371452114</v>
       </c>
       <c r="L41" s="9">
         <f t="shared" si="8"/>
-        <v>6.9895479355609649E-2</v>
+        <v>3.6830282139472738E-2</v>
       </c>
       <c r="M41" s="9">
         <f t="shared" si="8"/>
-        <v>0.1332890536548835</v>
+        <v>8.8693332499138411E-2</v>
       </c>
       <c r="N41" s="9">
         <f t="shared" si="8"/>
-        <v>4.2262382866182578E-2</v>
+        <v>1.9542598686250835E-2</v>
       </c>
       <c r="O41" s="9">
         <f t="shared" si="8"/>
-        <v>6.3544781393607239E-2</v>
+        <v>5.3397006300501697E-2</v>
       </c>
       <c r="P41" s="9">
         <f t="shared" si="8"/>
-        <v>4.0296690639848497E-2</v>
+        <v>2.353088413242448E-2</v>
       </c>
       <c r="Q41" s="9">
         <f t="shared" si="8"/>
-        <v>6.388499735585737E-3</v>
+        <v>2.5923855400128665E-3</v>
       </c>
     </row>
     <row r="42" spans="1:18">
@@ -2282,80 +2272,80 @@
       </c>
       <c r="C42" s="16">
         <f t="shared" si="8"/>
-        <v>7.759191176470587</v>
+        <v>11.110552763819097</v>
       </c>
       <c r="D42" s="16">
         <f t="shared" si="8"/>
-        <v>43.724221831589773</v>
+        <v>32.802584350323052</v>
       </c>
       <c r="E42" s="16">
         <f t="shared" si="8"/>
-        <v>7.6428517835705696</v>
+        <v>4.7135678391959814</v>
       </c>
       <c r="F42" s="16">
         <f t="shared" si="8"/>
-        <v>7.287370305264961</v>
+        <v>5.675520459440059</v>
       </c>
       <c r="G42" s="16">
         <f t="shared" si="8"/>
-        <v>2.3106296089864515</v>
+        <v>1.2505384063173008</v>
       </c>
       <c r="H42" s="16">
         <f t="shared" si="8"/>
-        <v>68.039663720548603</v>
+        <v>79.237411547533625</v>
       </c>
       <c r="I42" s="16">
         <f t="shared" si="8"/>
-        <v>23.786223902305608</v>
+        <v>22.77204202832344</v>
       </c>
       <c r="J42" s="16">
         <f t="shared" si="8"/>
-        <v>22.679887906849533</v>
+        <v>27.41939754430782</v>
       </c>
       <c r="K42" s="16">
         <f t="shared" si="8"/>
-        <v>7.1911839704644871</v>
+        <v>6.0415621707796889</v>
       </c>
       <c r="L42" s="16">
         <f t="shared" si="8"/>
-        <v>2.0788772922746777</v>
+        <v>1.6361144565804233</v>
       </c>
       <c r="M42" s="16">
         <f t="shared" si="8"/>
-        <v>3.9643706503842688</v>
+        <v>3.9400307321732639</v>
       </c>
       <c r="N42" s="16">
         <f t="shared" si="8"/>
-        <v>1.2569955720730608</v>
+        <v>0.86814236471614292</v>
       </c>
       <c r="O42" s="16">
         <f t="shared" si="8"/>
-        <v>1.8899906589041273</v>
+        <v>2.3720593183492102</v>
       </c>
       <c r="P42" s="16">
         <f t="shared" si="8"/>
-        <v>1.1985306617440814</v>
+        <v>1.0453142758827025</v>
       </c>
       <c r="Q42" s="16">
         <f t="shared" si="8"/>
-        <v>0.1900109585691836</v>
+        <v>0.11516174225826387</v>
       </c>
     </row>
     <row r="45" spans="1:18" ht="18" thickBot="1">
-      <c r="A45" s="23" t="s">
+      <c r="A45" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="B45" s="23"/>
-      <c r="C45" s="23"/>
-      <c r="D45" s="23"/>
-      <c r="E45" s="23"/>
+      <c r="B45" s="24"/>
+      <c r="C45" s="24"/>
+      <c r="D45" s="24"/>
+      <c r="E45" s="24"/>
     </row>
     <row r="46" spans="1:18" ht="17.25" thickTop="1"/>
     <row r="47" spans="1:18" ht="17.25" thickBot="1">
-      <c r="A47" s="25" t="s">
+      <c r="A47" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="B47" s="25"/>
+      <c r="B47" s="26"/>
       <c r="C47" s="2" t="s">
         <v>13</v>
       </c>
@@ -2745,10 +2735,10 @@
       </c>
     </row>
     <row r="55" spans="1:18" ht="17.25" thickBot="1">
-      <c r="A55" s="24" t="s">
+      <c r="A55" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="B55" s="24"/>
+      <c r="B55" s="25"/>
       <c r="C55" s="2" t="s">
         <v>13</v>
       </c>
@@ -2862,7 +2852,7 @@
         <f t="shared" si="11"/>
         <v>5.0526315789473683E-5</v>
       </c>
-      <c r="R56" s="26">
+      <c r="R56" s="23">
         <f t="shared" ref="R56:R60" si="12">SUM(C56:Q56)</f>
         <v>0.18204631578947369</v>
       </c>
@@ -2931,7 +2921,7 @@
         <f t="shared" si="13"/>
         <v>8.4210526315789476E-5</v>
       </c>
-      <c r="R57" s="26">
+      <c r="R57" s="23">
         <f t="shared" si="12"/>
         <v>0.64736000000000005</v>
       </c>
@@ -3000,7 +2990,7 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="R58" s="26">
+      <c r="R58" s="23">
         <f t="shared" si="12"/>
         <v>6.2534736842105254E-2</v>
       </c>
@@ -3069,7 +3059,7 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="R59" s="26">
+      <c r="R59" s="23">
         <f t="shared" si="12"/>
         <v>0.10583578947368422</v>
       </c>
@@ -3138,7 +3128,7 @@
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="R60" s="26">
+      <c r="R60" s="23">
         <f t="shared" si="12"/>
         <v>2.2231578947368423E-3</v>
       </c>
@@ -3213,10 +3203,10 @@
       </c>
     </row>
     <row r="64" spans="1:18" ht="18" thickBot="1">
-      <c r="A64" s="23" t="s">
+      <c r="A64" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="B64" s="23"/>
+      <c r="B64" s="24"/>
     </row>
     <row r="65" spans="2:21" ht="17.25" thickTop="1"/>
     <row r="66" spans="2:21">
@@ -3273,47 +3263,47 @@
       <c r="B67" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C67" s="19">
-        <v>1.2317E-4</v>
+      <c r="C67" s="22">
+        <v>3.5451000000000002E-6</v>
       </c>
       <c r="D67" s="19">
-        <v>1</v>
+        <v>3.4616000000000001E-2</v>
       </c>
       <c r="E67" s="19">
-        <v>0.42236000000000001</v>
+        <v>1</v>
       </c>
       <c r="F67" s="19">
-        <v>1</v>
+        <v>0.19928000000000001</v>
       </c>
       <c r="G67" s="19">
         <v>1</v>
       </c>
       <c r="H67" s="19">
-        <v>0.21027999999999999</v>
+        <v>0.45846999999999999</v>
       </c>
       <c r="I67" s="19">
-        <v>0.64142999999999994</v>
+        <v>0.53147999999999995</v>
       </c>
       <c r="J67" s="19">
-        <v>0.34044000000000002</v>
+        <v>1</v>
       </c>
       <c r="K67" s="19">
         <v>1</v>
       </c>
       <c r="L67" s="19">
-        <v>2.6764E-2</v>
-      </c>
-      <c r="M67" s="19">
-        <v>2.4316999999999999E-4</v>
+        <v>2.3508000000000001E-2</v>
+      </c>
+      <c r="M67" s="22">
+        <v>9.9125999999999999E-5</v>
       </c>
       <c r="N67" s="19">
         <v>1</v>
       </c>
       <c r="O67" s="19">
-        <v>2.6112E-2</v>
+        <v>1.9701E-2</v>
       </c>
       <c r="P67" s="22">
-        <v>3.1198000000000002E-6</v>
+        <v>3.6822999999999999E-4</v>
       </c>
       <c r="Q67" s="19">
         <v>1</v>
@@ -3327,46 +3317,46 @@
         <v>29</v>
       </c>
       <c r="C68" s="19">
-        <v>0.3856</v>
+        <v>0.39478999999999997</v>
       </c>
       <c r="D68" s="19">
-        <v>0.12464</v>
+        <v>0.42201</v>
       </c>
       <c r="E68" s="19">
-        <v>1</v>
+        <v>0.49748999999999999</v>
       </c>
       <c r="F68" s="19">
-        <v>0.13782</v>
+        <v>7.1894E-2</v>
       </c>
       <c r="G68" s="19">
-        <v>2.5465999999999999E-2</v>
+        <v>1</v>
       </c>
       <c r="H68" s="19">
-        <v>0.15301000000000001</v>
+        <v>1.0757E-3</v>
       </c>
       <c r="I68" s="19">
-        <v>0.20957000000000001</v>
+        <v>8.8457999999999995E-2</v>
       </c>
       <c r="J68" s="19">
-        <v>0.33278000000000002</v>
+        <v>0.22681000000000001</v>
       </c>
       <c r="K68" s="19">
-        <v>1.9358E-4</v>
+        <v>0.63590000000000002</v>
       </c>
       <c r="L68" s="19">
-        <v>3.6526000000000001E-4</v>
+        <v>2.32E-3</v>
       </c>
       <c r="M68" s="19">
-        <v>8.4378999999999996E-2</v>
+        <v>0.52734999999999999</v>
       </c>
       <c r="N68" s="19">
         <v>1</v>
       </c>
       <c r="O68" s="19">
-        <v>1.0204E-2</v>
+        <v>3.3514000000000002E-2</v>
       </c>
       <c r="P68" s="19">
-        <v>8.2170999999999998E-3</v>
+        <v>0.17765</v>
       </c>
       <c r="Q68" s="19">
         <v>1</v>
@@ -3386,31 +3376,31 @@
         <v>30</v>
       </c>
       <c r="C69" s="19">
-        <v>0.13777</v>
+        <v>0.21387</v>
       </c>
       <c r="D69" s="19">
-        <v>0.14624999999999999</v>
+        <v>6.9061999999999998E-2</v>
       </c>
       <c r="E69" s="19">
         <v>1</v>
       </c>
       <c r="F69" s="19">
-        <v>8.6062E-2</v>
+        <v>0.19481999999999999</v>
       </c>
       <c r="G69" s="19">
         <v>1</v>
       </c>
       <c r="H69" s="19">
-        <v>0.33423000000000003</v>
+        <v>0.20172000000000001</v>
       </c>
       <c r="I69" s="19">
-        <v>0.27295000000000003</v>
+        <v>8.7661000000000003E-2</v>
       </c>
       <c r="J69" s="19">
-        <v>0.27182000000000001</v>
+        <v>0.12146999999999999</v>
       </c>
       <c r="K69" s="19">
-        <v>3.8524000000000002E-3</v>
+        <v>0.19097</v>
       </c>
       <c r="L69" s="19">
         <v>1</v>
@@ -3448,7 +3438,7 @@
         <v>1</v>
       </c>
       <c r="D70" s="19">
-        <v>2.4666E-2</v>
+        <v>1.1858E-2</v>
       </c>
       <c r="E70" s="19">
         <v>1</v>
@@ -3457,25 +3447,25 @@
         <v>1</v>
       </c>
       <c r="G70" s="19">
-        <v>6.6237999999999996E-4</v>
+        <v>2.5447000000000001E-2</v>
       </c>
       <c r="H70" s="19">
-        <v>0.33431</v>
+        <v>0.33783000000000002</v>
       </c>
       <c r="I70" s="19">
-        <v>8.2947000000000007E-2</v>
+        <v>0.52734999999999999</v>
       </c>
       <c r="J70" s="19">
-        <v>0.27313999999999999</v>
+        <v>0.124</v>
       </c>
       <c r="K70" s="19">
-        <v>5.0339E-3</v>
+        <v>0.17765</v>
       </c>
       <c r="L70" s="19">
         <v>1</v>
       </c>
       <c r="M70" s="22">
-        <v>6.6717999999999996E-10</v>
+        <v>2.9058E-7</v>
       </c>
       <c r="N70" s="19">
         <v>1</v>
@@ -3484,7 +3474,7 @@
         <v>1</v>
       </c>
       <c r="P70" s="22">
-        <v>2.2337E-5</v>
+        <v>7.3923000000000001E-3</v>
       </c>
       <c r="Q70" s="19">
         <v>1</v>
@@ -3507,7 +3497,7 @@
         <v>1</v>
       </c>
       <c r="D71" s="19">
-        <v>5.0339E-3</v>
+        <v>1</v>
       </c>
       <c r="E71" s="19">
         <v>1</v>
@@ -3519,7 +3509,7 @@
         <v>1</v>
       </c>
       <c r="H71" s="19">
-        <v>1.661E-2</v>
+        <v>0.52932000000000001</v>
       </c>
       <c r="I71" s="19">
         <v>1</v>
@@ -3563,46 +3553,46 @@
         <v>33</v>
       </c>
       <c r="C72" s="19">
-        <v>0.20197999999999999</v>
+        <v>0.20069999999999999</v>
       </c>
       <c r="D72" s="19">
-        <v>1.8086999999999999E-2</v>
+        <v>0.12712000000000001</v>
       </c>
       <c r="E72" s="19">
-        <v>0.22611999999999999</v>
+        <v>7.3043999999999998E-2</v>
       </c>
       <c r="F72" s="19">
-        <v>0.17748</v>
+        <v>9.7156000000000006E-2</v>
       </c>
       <c r="G72" s="19">
-        <v>7.6411999999999999E-3</v>
+        <v>1</v>
       </c>
       <c r="H72" s="19">
-        <v>0.51849000000000001</v>
+        <v>7.1541E-3</v>
       </c>
       <c r="I72" s="19">
-        <v>0.14258999999999999</v>
+        <v>5.0233E-2</v>
       </c>
       <c r="J72" s="19">
-        <v>2.9485000000000001E-2</v>
+        <v>1.1205E-2</v>
       </c>
       <c r="K72" s="22">
-        <v>6.1221000000000002E-5</v>
+        <v>1</v>
       </c>
       <c r="L72" s="19">
-        <v>5.6605000000000002E-4</v>
+        <v>5.2781E-3</v>
       </c>
       <c r="M72" s="22">
-        <v>5.2994000000000005E-7</v>
+        <v>5.4635999999999997E-5</v>
       </c>
       <c r="N72" s="19">
-        <v>1</v>
+        <v>0.41596</v>
       </c>
       <c r="O72" s="19">
-        <v>1.1351E-2</v>
+        <v>4.2472999999999997E-2</v>
       </c>
       <c r="P72" s="22">
-        <v>1.1163E-6</v>
+        <v>7.4916999999999996E-3</v>
       </c>
       <c r="Q72" s="19">
         <v>1</v>
@@ -3661,19 +3651,19 @@
       </c>
       <c r="C75" s="21">
         <f>1/C67</f>
-        <v>8118.8601120402691</v>
+        <v>282079.49000028207</v>
       </c>
       <c r="D75" s="21">
         <f t="shared" ref="D75:Q75" si="18">1/D67</f>
-        <v>1</v>
+        <v>28.888375317772127</v>
       </c>
       <c r="E75" s="21">
         <f t="shared" si="18"/>
-        <v>2.3676484515579128</v>
+        <v>1</v>
       </c>
       <c r="F75" s="21">
         <f t="shared" si="18"/>
-        <v>1</v>
+        <v>5.0180650341228423</v>
       </c>
       <c r="G75" s="21">
         <f t="shared" si="18"/>
@@ -3681,15 +3671,15 @@
       </c>
       <c r="H75" s="21">
         <f t="shared" si="18"/>
-        <v>4.7555640098915735</v>
+        <v>2.1811677972386416</v>
       </c>
       <c r="I75" s="21">
         <f t="shared" si="18"/>
-        <v>1.5590165723461642</v>
+        <v>1.8815383457514865</v>
       </c>
       <c r="J75" s="21">
         <f t="shared" si="18"/>
-        <v>2.9373751615556336</v>
+        <v>1</v>
       </c>
       <c r="K75" s="21">
         <f t="shared" si="18"/>
@@ -3697,11 +3687,11 @@
       </c>
       <c r="L75" s="21">
         <f t="shared" si="18"/>
-        <v>37.363622776864446</v>
+        <v>42.538710226305938</v>
       </c>
       <c r="M75" s="21">
         <f t="shared" si="18"/>
-        <v>4112.3493852037673</v>
+        <v>10088.170611141375</v>
       </c>
       <c r="N75" s="21">
         <f t="shared" si="18"/>
@@ -3709,11 +3699,11 @@
       </c>
       <c r="O75" s="21">
         <f t="shared" si="18"/>
-        <v>38.296568627450981</v>
+        <v>50.758844728693973</v>
       </c>
       <c r="P75" s="21">
         <f t="shared" si="18"/>
-        <v>320533.36752355919</v>
+        <v>2715.6939956005758</v>
       </c>
       <c r="Q75" s="21">
         <f t="shared" si="18"/>
@@ -3726,47 +3716,47 @@
       </c>
       <c r="C76" s="21">
         <f t="shared" ref="C76:Q76" si="19">1/C68</f>
-        <v>2.5933609958506225</v>
+        <v>2.5329922237138733</v>
       </c>
       <c r="D76" s="21">
         <f t="shared" si="19"/>
-        <v>8.0231065468549421</v>
+        <v>2.3696120945001304</v>
       </c>
       <c r="E76" s="21">
         <f t="shared" si="19"/>
-        <v>1</v>
+        <v>2.0100906550885447</v>
       </c>
       <c r="F76" s="21">
         <f t="shared" si="19"/>
-        <v>7.2558409519663334</v>
+        <v>13.909366567446519</v>
       </c>
       <c r="G76" s="21">
         <f t="shared" si="19"/>
-        <v>39.268043666064557</v>
+        <v>1</v>
       </c>
       <c r="H76" s="21">
         <f t="shared" si="19"/>
-        <v>6.5355205542121428</v>
+        <v>929.62721948498654</v>
       </c>
       <c r="I76" s="21">
         <f t="shared" si="19"/>
-        <v>4.7716753352101922</v>
+        <v>11.304800018087681</v>
       </c>
       <c r="J76" s="21">
         <f t="shared" si="19"/>
-        <v>3.0049882805457058</v>
+        <v>4.4089766765133813</v>
       </c>
       <c r="K76" s="21">
         <f t="shared" si="19"/>
-        <v>5165.8229155904537</v>
+        <v>1.5725743041358704</v>
       </c>
       <c r="L76" s="21">
         <f t="shared" si="19"/>
-        <v>2737.7758309149644</v>
+        <v>431.0344827586207</v>
       </c>
       <c r="M76" s="21">
         <f t="shared" si="19"/>
-        <v>11.851290012917907</v>
+        <v>1.8962738219398882</v>
       </c>
       <c r="N76" s="21">
         <f t="shared" si="19"/>
@@ -3774,11 +3764,11 @@
       </c>
       <c r="O76" s="21">
         <f t="shared" si="19"/>
-        <v>98.000784006272056</v>
+        <v>29.838276541146982</v>
       </c>
       <c r="P76" s="21">
         <f t="shared" si="19"/>
-        <v>121.69743583502697</v>
+        <v>5.6290458767238949</v>
       </c>
       <c r="Q76" s="21">
         <f t="shared" si="19"/>
@@ -3791,11 +3781,11 @@
       </c>
       <c r="C77" s="21">
         <f t="shared" ref="C77:Q77" si="20">1/C69</f>
-        <v>7.2584742687087171</v>
+        <v>4.6757375976060223</v>
       </c>
       <c r="D77" s="21">
         <f t="shared" si="20"/>
-        <v>6.8376068376068382</v>
+        <v>14.479742839767166</v>
       </c>
       <c r="E77" s="21">
         <f t="shared" si="20"/>
@@ -3803,7 +3793,7 @@
       </c>
       <c r="F77" s="21">
         <f t="shared" si="20"/>
-        <v>11.619530106202506</v>
+        <v>5.1329432296478803</v>
       </c>
       <c r="G77" s="21">
         <f t="shared" si="20"/>
@@ -3811,19 +3801,19 @@
       </c>
       <c r="H77" s="21">
         <f t="shared" si="20"/>
-        <v>2.9919516500613348</v>
+        <v>4.9573666468372002</v>
       </c>
       <c r="I77" s="21">
         <f t="shared" si="20"/>
-        <v>3.6636746656896864</v>
+        <v>11.407581478650711</v>
       </c>
       <c r="J77" s="21">
         <f t="shared" si="20"/>
-        <v>3.6789051578250311</v>
+        <v>8.2324853873384374</v>
       </c>
       <c r="K77" s="21">
         <f t="shared" si="20"/>
-        <v>259.57844460595993</v>
+        <v>5.236424569304079</v>
       </c>
       <c r="L77" s="21">
         <f t="shared" si="20"/>
@@ -3860,7 +3850,7 @@
       </c>
       <c r="D78" s="21">
         <f t="shared" si="21"/>
-        <v>40.541636260439468</v>
+        <v>84.331253162421987</v>
       </c>
       <c r="E78" s="21">
         <f t="shared" si="21"/>
@@ -3872,23 +3862,23 @@
       </c>
       <c r="G78" s="21">
         <f t="shared" si="21"/>
-        <v>1509.7074187022556</v>
+        <v>39.297363146932838</v>
       </c>
       <c r="H78" s="21">
         <f t="shared" si="21"/>
-        <v>2.9912356794591846</v>
+        <v>2.9600686735932271</v>
       </c>
       <c r="I78" s="21">
         <f t="shared" si="21"/>
-        <v>12.055891111191483</v>
+        <v>1.8962738219398882</v>
       </c>
       <c r="J78" s="21">
         <f t="shared" si="21"/>
-        <v>3.6611261624075566</v>
+        <v>8.064516129032258</v>
       </c>
       <c r="K78" s="21">
         <f t="shared" si="21"/>
-        <v>198.65313176662229</v>
+        <v>5.6290458767238949</v>
       </c>
       <c r="L78" s="21">
         <f t="shared" si="21"/>
@@ -3896,7 +3886,7 @@
       </c>
       <c r="M78" s="21">
         <f t="shared" si="21"/>
-        <v>1498845888.6657274</v>
+        <v>3441393.0759171313</v>
       </c>
       <c r="N78" s="21">
         <f t="shared" si="21"/>
@@ -3908,7 +3898,7 @@
       </c>
       <c r="P78" s="21">
         <f t="shared" si="21"/>
-        <v>44768.769306531765</v>
+        <v>135.2758951882364</v>
       </c>
       <c r="Q78" s="21">
         <f t="shared" si="21"/>
@@ -3925,7 +3915,7 @@
       </c>
       <c r="D79" s="21">
         <f t="shared" si="22"/>
-        <v>198.65313176662229</v>
+        <v>1</v>
       </c>
       <c r="E79" s="21">
         <f t="shared" si="22"/>
@@ -3941,7 +3931,7 @@
       </c>
       <c r="H79" s="21">
         <f t="shared" si="22"/>
-        <v>60.204695966285371</v>
+        <v>1.8892163530567521</v>
       </c>
       <c r="I79" s="21">
         <f t="shared" si="22"/>
@@ -3986,59 +3976,59 @@
       </c>
       <c r="C80" s="21">
         <f t="shared" si="22"/>
-        <v>4.9509852460639667</v>
+        <v>4.9825610363726955</v>
       </c>
       <c r="D80" s="21">
         <f t="shared" si="22"/>
-        <v>55.288328633825401</v>
+        <v>7.8665827564505975</v>
       </c>
       <c r="E80" s="21">
         <f t="shared" si="22"/>
-        <v>4.4224305678400855</v>
+        <v>13.690378402059034</v>
       </c>
       <c r="F80" s="21">
         <f t="shared" si="22"/>
-        <v>5.6344376831192244</v>
+        <v>10.292725101897977</v>
       </c>
       <c r="G80" s="21">
         <f t="shared" si="22"/>
-        <v>130.86949693765376</v>
+        <v>1</v>
       </c>
       <c r="H80" s="21">
         <f t="shared" si="22"/>
-        <v>1.9286775058342494</v>
+        <v>139.77998630156134</v>
       </c>
       <c r="I80" s="21">
         <f t="shared" si="22"/>
-        <v>7.01311452416018</v>
+        <v>19.907232297493678</v>
       </c>
       <c r="J80" s="21">
         <f t="shared" si="22"/>
-        <v>33.915550279803291</v>
+        <v>89.245872378402495</v>
       </c>
       <c r="K80" s="21">
         <f t="shared" si="22"/>
-        <v>16334.264386403358</v>
+        <v>1</v>
       </c>
       <c r="L80" s="21">
         <f t="shared" si="22"/>
-        <v>1766.6283897182227</v>
+        <v>189.46211704969591</v>
       </c>
       <c r="M80" s="21">
         <f t="shared" si="22"/>
-        <v>1887006.076159565</v>
+        <v>18302.950435610222</v>
       </c>
       <c r="N80" s="21">
         <f t="shared" si="22"/>
-        <v>1</v>
+        <v>2.4040773151264543</v>
       </c>
       <c r="O80" s="21">
         <f t="shared" si="22"/>
-        <v>88.097964937009962</v>
+        <v>23.544369364066586</v>
       </c>
       <c r="P80" s="21">
         <f t="shared" si="22"/>
-        <v>895816.53677326883</v>
+        <v>133.48105236461686</v>
       </c>
       <c r="Q80" s="21">
         <f t="shared" si="22"/>
@@ -4058,21 +4048,21 @@
     <mergeCell ref="A55:B55"/>
   </mergeCells>
   <conditionalFormatting sqref="C67:Q72">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
       <formula>0.000063342484</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="lessThan">
       <formula>0.002699796063</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="lessThan">
       <formula>0.045500263896</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="lessThan">
       <formula>0.317310507863</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C75:Q80">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>370</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>